<commit_message>
upload total video scripts
</commit_message>
<xml_diff>
--- a/Doc/视频脚本.xlsx
+++ b/Doc/视频脚本.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="5910" activeTab="1"/>
+    <workbookView windowWidth="14400" windowHeight="12280" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="概览篇" sheetId="1" r:id="rId1"/>
     <sheet name="实现篇" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="通信篇" sheetId="3" r:id="rId3"/>
+    <sheet name="上位机篇" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="295">
   <si>
     <t>脚本场景</t>
   </si>
@@ -481,6 +481,499 @@
   </si>
   <si>
     <t>e_v3.wav</t>
+  </si>
+  <si>
+    <t>小白学习pid环控制-实现篇(无字幕).mp4</t>
+  </si>
+  <si>
+    <t>在上一篇章中，我通过将概览篇的提到的关键驱动代码进行了整合。</t>
+  </si>
+  <si>
+    <t>然后将pid仿真网页中的算法移植到了单片机中</t>
+  </si>
+  <si>
+    <t>最后综合了编码器，步进驱动器，以及算法。
+实现了游标运动的环控制功能</t>
+  </si>
+  <si>
+    <t>saleae logic.png | SerialStudio数据详情.jpg</t>
+  </si>
+  <si>
+    <t>在这一章节中，我将开始适配通信代码并将代码重构
+以更好的满足一些通信的要求</t>
+  </si>
+  <si>
+    <t>标题: 小白学习pid环控制-通信篇</t>
+  </si>
+  <si>
+    <t>所以，欢迎来到小白学习pid环控制，通信的内容。</t>
+  </si>
+  <si>
+    <t>s_v5.wav</t>
+  </si>
+  <si>
+    <t>辅助工具</t>
+  </si>
+  <si>
+    <t>SerialStudio</t>
+  </si>
+  <si>
+    <t>SerialStudio介绍.mp4</t>
+  </si>
+  <si>
+    <t>首先需要安装几个辅助工具，来更好的帮助后续的开发</t>
+  </si>
+  <si>
+    <t>s_s_v1.wav</t>
+  </si>
+  <si>
+    <t>第一个辅助工具是Serial Studio，我们需要编译它的开源版本。</t>
+  </si>
+  <si>
+    <t>s_s_v2.wav</t>
+  </si>
+  <si>
+    <t>Qt依赖1.jpg</t>
+  </si>
+  <si>
+    <t>根据官方指导，我们需要安装Qt的开发环境</t>
+  </si>
+  <si>
+    <t>s_s_v3.wav</t>
+  </si>
+  <si>
+    <t>Qt依赖2.jpg | 编译SerialStudio.jpg</t>
+  </si>
+  <si>
+    <t>按照如图所示，勾选Qt Online Installer的依赖项目。
+在安装完成后打开项目，并勾选编译器</t>
+  </si>
+  <si>
+    <t>s_s_v4.wav</t>
+  </si>
+  <si>
+    <t>SerialStudio 启动脚本.jpg</t>
+  </si>
+  <si>
+    <t>并按照类似的环境变量设置方式，即可启动程序</t>
+  </si>
+  <si>
+    <t>s_s_v5.wav</t>
+  </si>
+  <si>
+    <t>Logic 2</t>
+  </si>
+  <si>
+    <t>Logic介绍.mp4</t>
+  </si>
+  <si>
+    <t>接下来我们将要安装逻辑分析仪上位机程序，
+在它的帮助下可以很方便的看到通信的内容</t>
+  </si>
+  <si>
+    <t>s_s_v6.wav</t>
+  </si>
+  <si>
+    <t>测试代码</t>
+  </si>
+  <si>
+    <t>SerialStudio数据详情.jpg</t>
+  </si>
+  <si>
+    <t>接下来我们要开始编写测试代码，以测试当前的通信是否符合期待</t>
+  </si>
+  <si>
+    <t>硬件接线.jpeg | 串口模块.png</t>
+  </si>
+  <si>
+    <t>首先按照图中所示完成通信模块的接线，然后开始编写通信代码</t>
+  </si>
+  <si>
+    <t>t_v2.wav</t>
+  </si>
+  <si>
+    <t>串口模式使用.jpg | 通信代码1.jpg | 通信代码2.jpg</t>
+  </si>
+  <si>
+    <t>保障一个良好的通信是比较困难的，示例只保证了如下内容：
+确保接收到数据，确认通信时延，保障数据格式</t>
+  </si>
+  <si>
+    <t>t_v3.wav</t>
+  </si>
+  <si>
+    <t>数据接收.jpeg</t>
+  </si>
+  <si>
+    <t>对于确保接收，我们需要下位机每次对命令进行回复</t>
+  </si>
+  <si>
+    <t>t_v4.wav</t>
+  </si>
+  <si>
+    <t>通信时延.jpeg</t>
+  </si>
+  <si>
+    <t>对于通信时延，则跟实际状态有关，我们用于控制上位机
+的指令发送速度，以降低脏数据的出现频率</t>
+  </si>
+  <si>
+    <t>t_v5.wav</t>
+  </si>
+  <si>
+    <t>格式确认.jpeg</t>
+  </si>
+  <si>
+    <t>我们让每个命令都有明确的数据格式，保障了解析的成功率，并使得上位机能够根据回复内容区分是否为脏数据</t>
+  </si>
+  <si>
+    <t>t_v6.wav</t>
+  </si>
+  <si>
+    <t>逻辑重构</t>
+  </si>
+  <si>
+    <t>代码重构.jpg</t>
+  </si>
+  <si>
+    <t>在上述的基础上，我们就可以开始重构下位机了</t>
+  </si>
+  <si>
+    <t>l_re_v1.wav</t>
+  </si>
+  <si>
+    <t>等待逻辑.jpg</t>
+  </si>
+  <si>
+    <t>为了让通信每次都有回复且间隔不至于太长，我们就不能使用长时间
+等待的方式，等待电机到指定位置</t>
+  </si>
+  <si>
+    <t>l_re_v2.wav</t>
+  </si>
+  <si>
+    <t>电机1-设定变量.jpg | 电机2-交给定时器.jpg</t>
+  </si>
+  <si>
+    <t>我们把逻辑拆分为设定以及定时器执行，
+让主逻辑可以一直执行不受阻断</t>
+  </si>
+  <si>
+    <t>l_re_v3.wav</t>
+  </si>
+  <si>
+    <t>通信1-字节接收中断.jpg</t>
+  </si>
+  <si>
+    <t>对于命令接收逻辑，接收中断只完成字节接收，以及少量逻辑判断</t>
+  </si>
+  <si>
+    <t>l_re_v4.wav</t>
+  </si>
+  <si>
+    <t>通信2-命令处理主循环.jpg</t>
+  </si>
+  <si>
+    <t>对于主循环，接收到命令首先立刻回复。然后只有
+执行完当前命令才会清空缓冲，接收下一条命令</t>
+  </si>
+  <si>
+    <t>l_re_v5.wav</t>
+  </si>
+  <si>
+    <t>逻辑概览.mp4</t>
+  </si>
+  <si>
+    <t>对于全部逻辑，推荐还是从仓库以及博客进行查询</t>
+  </si>
+  <si>
+    <t>l_re_v6.wav</t>
+  </si>
+  <si>
+    <t>知识概览.mp4</t>
+  </si>
+  <si>
+    <t>在这一篇章中，我们安装了调试通讯所需的辅助软件，
+然后经历了接线、测试代码编写</t>
+  </si>
+  <si>
+    <t>最后在上面的基础上，重构了下位机的整体代码，
+以满足了通信所需的基础要求</t>
+  </si>
+  <si>
+    <t>下一篇章将开始封装上位机，以完整联通这套逻辑</t>
+  </si>
+  <si>
+    <t>e_v4.wav</t>
+  </si>
+  <si>
+    <t>金閉開羅巧夢
+Sentence know.mp3</t>
+  </si>
+  <si>
+    <t>小白学习pid环控制-通讯篇(无字幕).mp4</t>
+  </si>
+  <si>
+    <t>这一节是小白学习pid环控制的最后一章，
+我们首先对前面的内容进行一个回顾</t>
+  </si>
+  <si>
+    <t>在概览篇中，我从认识关键部件开始并逐步添加驱动代码</t>
+  </si>
+  <si>
+    <t>在实现篇中，我们组合了级联pid算法以及驱动代码，完成了电机运动控制</t>
+  </si>
+  <si>
+    <t>在通讯篇中，我们使用协议分析仪，完善了下位机通讯
+并重构了整体代码</t>
+  </si>
+  <si>
+    <t>total.mp4</t>
+  </si>
+  <si>
+    <t>那么欢迎来到小白学习pid环控制 上位机篇的内容</t>
+  </si>
+  <si>
+    <t>在这一节中，将封装上述的所有逻辑以实现交互功能</t>
+  </si>
+  <si>
+    <t>s_v6.wav</t>
+  </si>
+  <si>
+    <t>最小ui设计</t>
+  </si>
+  <si>
+    <t>概念ui设计.jpg</t>
+  </si>
+  <si>
+    <t>顶层交互是一个很空泛的概念，所以我们从对设备最基础的控制进行实现</t>
+  </si>
+  <si>
+    <t>m_u_v1.wav</t>
+  </si>
+  <si>
+    <t>将基础功能输入ai，得到概念设计图</t>
+  </si>
+  <si>
+    <t>m_u_v2.wav</t>
+  </si>
+  <si>
+    <t>design studio.mp4</t>
+  </si>
+  <si>
+    <t>然后我们打开Design Studio对于实现进行细化</t>
+  </si>
+  <si>
+    <t>m_u_v3.wav</t>
+  </si>
+  <si>
+    <t>包含大致布局，需要定制哪些组件，得到程序编码前期稿</t>
+  </si>
+  <si>
+    <t>m_u_v4.wav</t>
+  </si>
+  <si>
+    <t>在最小实现中，需要定义一个滑动组件显示编码器读数，
+以及位置设定组件还有测速组件</t>
+  </si>
+  <si>
+    <t>m_u_v5.wav</t>
+  </si>
+  <si>
+    <t>逻辑组装</t>
+  </si>
+  <si>
+    <t>找到串口通信设备.jpg</t>
+  </si>
+  <si>
+    <t>有了需要实现的目标后，开始填充软件模块逻辑</t>
+  </si>
+  <si>
+    <t>l_v1.wav</t>
+  </si>
+  <si>
+    <t>首先实现串口通信的部分</t>
+  </si>
+  <si>
+    <t>l_v2.wav</t>
+  </si>
+  <si>
+    <t>串口基础读写.jpg</t>
+  </si>
+  <si>
+    <t>我们需要实现一个找到串口模块的功能,并实现基础读写</t>
+  </si>
+  <si>
+    <t>l_v3.wav</t>
+  </si>
+  <si>
+    <t>二级封装类.png | 数据判断.jpg</t>
+  </si>
+  <si>
+    <t>接着封装二级协议类，并实现一个命令队列
+控制整体的收发速率以及上报当前命令是否正常解析的功能</t>
+  </si>
+  <si>
+    <t>l_v4.wav</t>
+  </si>
+  <si>
+    <t>简易测试Demo.jpg</t>
+  </si>
+  <si>
+    <t>在正式和界面代码联调前，我们编写简易Demo进行测试</t>
+  </si>
+  <si>
+    <t>l_v5.wav</t>
+  </si>
+  <si>
+    <t>简易测试Demo2.jpg</t>
+  </si>
+  <si>
+    <t>通过逐条点击指令，并查看逻辑分析仪上的数据情况进行模块调试</t>
+  </si>
+  <si>
+    <t>l_v5_2.wav</t>
+  </si>
+  <si>
+    <t>Qml Python配置.jpg</t>
+  </si>
+  <si>
+    <t>终于到了ui实际编写的阶段，我们要配置conda环境以使用Pyside6开发环境</t>
+  </si>
+  <si>
+    <t>l_v6.wav</t>
+  </si>
+  <si>
+    <t>Qml Python配置2.jpg | Qml Python配置3.jpg</t>
+  </si>
+  <si>
+    <t>这一步需要将conda环境添加到Creator的Python中，
+才能创建一个Qml Pyside6项目</t>
+  </si>
+  <si>
+    <t>l_v7.wav</t>
+  </si>
+  <si>
+    <t>Fluent介绍.png | Fluent介绍2.png</t>
+  </si>
+  <si>
+    <t>在此之前介绍一下Fluent UI项目</t>
+  </si>
+  <si>
+    <t>l_v8.wav</t>
+  </si>
+  <si>
+    <t>Fluent UI是一个大佬移植到Qml的界面库，后续程序也定制它进行开发</t>
+  </si>
+  <si>
+    <t>l_v9.wav</t>
+  </si>
+  <si>
+    <t>主窗口.png</t>
+  </si>
+  <si>
+    <t>详细的ui编写过程推荐对照仓库进行，这里放出大致的组装逻辑</t>
+  </si>
+  <si>
+    <t>l_v10.wav</t>
+  </si>
+  <si>
+    <t>封装Slider.png</t>
+  </si>
+  <si>
+    <t>首先封装Slider，使用三个Text组件对当前详细数值进行可视化
+并留出数据装填接口</t>
+  </si>
+  <si>
+    <t>l_v11.wav</t>
+  </si>
+  <si>
+    <t>位置组件.jpg</t>
+  </si>
+  <si>
+    <t>然后再次定制Slider组件，使其能够转换编码器输出到毫米距离
+并增加一个矩形框，强调其视觉效果并框定范围</t>
+  </si>
+  <si>
+    <t>l_v12.wav</t>
+  </si>
+  <si>
+    <t>速度组件.jpg</t>
+  </si>
+  <si>
+    <t>速度和位置组件同理，但速度组件会记录上一次调用的时间和数值
+并综合起来计算当前的毫米数值</t>
+  </si>
+  <si>
+    <t>l_v13.wav</t>
+  </si>
+  <si>
+    <t>按钮组件.jpg</t>
+  </si>
+  <si>
+    <t>最后定制一下按钮的样式，使得当前页面设定的数值可以交给串口通信类</t>
+  </si>
+  <si>
+    <t>l_v14.wav</t>
+  </si>
+  <si>
+    <t>相互调用.jpg</t>
+  </si>
+  <si>
+    <t>当然对于细节肯定会有疑惑，这里给出一个官方逻辑和ui代码连接的示例</t>
+  </si>
+  <si>
+    <t>l_v15.wav</t>
+  </si>
+  <si>
+    <t>通信设备1.png | 通信设备2.png</t>
+  </si>
+  <si>
+    <t>个人的核心逻辑如下，首先判断是否能正常打开通信设备</t>
+  </si>
+  <si>
+    <t>等待信号1.png | 等待信号2.png</t>
+  </si>
+  <si>
+    <t>然后发送一个询问信号，并等待返回</t>
+  </si>
+  <si>
+    <t>数据填写.png | 错误示例.png</t>
+  </si>
+  <si>
+    <t>可以通信后填写数据到界面中</t>
+  </si>
+  <si>
+    <t>然后点击按钮发送数据到通信对象</t>
+  </si>
+  <si>
+    <t>关闭程序时，清理程序资源</t>
+  </si>
+  <si>
+    <t>e_v5.wav</t>
+  </si>
+  <si>
+    <t>总结.mp4</t>
+  </si>
+  <si>
+    <t>经过上述步骤，我们成功将机械运动、电驱、指令、应用封装
+这一套逻辑实现了出来</t>
+  </si>
+  <si>
+    <t>e_v6.wav</t>
+  </si>
+  <si>
+    <t>很高兴最后还是完成了这样的一个东西，虽然是一个玩具水平，
+但足够用于练手串联碎片知识</t>
+  </si>
+  <si>
+    <t>e_v7.wav</t>
+  </si>
+  <si>
+    <t>最后期待着这四个部分能帮助想要入门全栈的朋友，那么我们未来再见啦</t>
+  </si>
+  <si>
+    <t>e_v8.wav</t>
   </si>
 </sst>
 </file>
@@ -502,15 +995,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FFE88D2F"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFE88D2F"/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1137,7 +1630,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1147,28 +1640,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1493,7 +1977,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="B30" sqref="B30:D30"/>
     </sheetView>
@@ -1508,13 +1992,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1522,7 +2006,7 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1530,10 +2014,10 @@
       </c>
     </row>
     <row r="3" ht="28" customHeight="1" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1541,7 +2025,7 @@
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.00555555555555556</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1549,7 +2033,7 @@
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1558,7 +2042,7 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>0.00763888888888889</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1574,7 +2058,7 @@
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>0.0104166666666667</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1582,7 +2066,7 @@
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="5"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1600,7 +2084,7 @@
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>0.0138888888888889</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1608,10 +2092,10 @@
       </c>
     </row>
     <row r="13" ht="28" spans="1:3">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>0.0145833333333333</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1619,7 +2103,7 @@
       </c>
     </row>
     <row r="14" ht="28" spans="3:4">
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1627,15 +2111,15 @@
       </c>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>0.0201388888888889</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" ht="28" spans="3:4">
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1643,15 +2127,15 @@
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>0.025</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" ht="28" spans="3:4">
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1659,15 +2143,15 @@
       </c>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>0.0305555555555556</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" ht="28" spans="3:4">
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1679,7 +2163,7 @@
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>0.0354166666666667</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1687,16 +2171,16 @@
       </c>
     </row>
     <row r="23" ht="42" spans="1:3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="4"/>
       <c r="C23" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" ht="28" spans="3:4">
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1704,10 +2188,10 @@
       </c>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>0.0402777777777778</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1720,7 +2204,7 @@
       </c>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <v>0.0430555555555556</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1728,7 +2212,7 @@
       </c>
     </row>
     <row r="28" ht="28" spans="3:4">
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1736,10 +2220,10 @@
       </c>
     </row>
     <row r="29" ht="28" spans="2:4">
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>0.05</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1747,12 +2231,12 @@
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="2:3">
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>0.0534722222222222</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1765,7 +2249,7 @@
       </c>
     </row>
     <row r="33" ht="28" spans="3:4">
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -1773,15 +2257,15 @@
       </c>
     </row>
     <row r="34" spans="2:3">
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>0.0583333333333333</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="35" ht="28" spans="3:4">
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1789,15 +2273,15 @@
       </c>
     </row>
     <row r="36" spans="2:3">
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>0.0645833333333333</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="37" ht="28" spans="3:4">
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -1805,15 +2289,15 @@
       </c>
     </row>
     <row r="38" spans="2:3">
-      <c r="B38" s="5">
+      <c r="B38" s="4">
         <v>0.06875</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="39" ht="28" spans="3:4">
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -1821,15 +2305,15 @@
       </c>
     </row>
     <row r="40" spans="2:3">
-      <c r="B40" s="5">
+      <c r="B40" s="4">
         <v>0.0736111111111111</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" ht="28" spans="3:4">
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -1837,12 +2321,12 @@
       </c>
     </row>
     <row r="42" spans="2:4">
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
     </row>
     <row r="43" spans="2:3">
-      <c r="B43" s="5">
+      <c r="B43" s="4">
         <v>0.0798611111111111</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1855,7 +2339,7 @@
       </c>
     </row>
     <row r="45" ht="42" spans="3:4">
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1863,7 +2347,7 @@
       </c>
     </row>
     <row r="46" spans="2:3">
-      <c r="B46" s="5">
+      <c r="B46" s="4">
         <v>0.0875</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1871,7 +2355,7 @@
       </c>
     </row>
     <row r="47" ht="28" spans="3:4">
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1879,7 +2363,7 @@
       </c>
     </row>
     <row r="48" spans="2:3">
-      <c r="B48" s="5">
+      <c r="B48" s="4">
         <v>0.0930555555555556</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -1904,7 +2388,7 @@
       </c>
     </row>
     <row r="52" spans="2:3">
-      <c r="B52" s="5">
+      <c r="B52" s="4">
         <v>0.0979166666666667</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -1920,7 +2404,7 @@
       </c>
     </row>
     <row r="54" spans="2:3">
-      <c r="B54" s="5">
+      <c r="B54" s="4">
         <v>0.103472222222222</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -1936,7 +2420,7 @@
       </c>
     </row>
     <row r="56" spans="2:3">
-      <c r="B56" s="5">
+      <c r="B56" s="4">
         <v>0.10625</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -1944,7 +2428,7 @@
       </c>
     </row>
     <row r="57" ht="28" spans="3:4">
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -1952,7 +2436,7 @@
       </c>
     </row>
     <row r="58" spans="2:3">
-      <c r="B58" s="5">
+      <c r="B58" s="4">
         <v>0.1125</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -1960,7 +2444,7 @@
       </c>
     </row>
     <row r="59" ht="28" spans="3:4">
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="5" t="s">
         <v>81</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -1968,7 +2452,7 @@
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="B60" s="5">
+      <c r="B60" s="4">
         <v>0.116666666666667</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -1988,7 +2472,7 @@
       <c r="A63" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B63" s="4">
         <v>0.119444444444444</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -2001,7 +2485,7 @@
       </c>
     </row>
     <row r="65" ht="56" spans="3:4">
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="5" t="s">
         <v>88</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2020,29 +2504,29 @@
   <sheetPr/>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="25.4545454545455" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.9090909090909" style="3" customWidth="1"/>
-    <col min="3" max="3" width="61.1818181818182" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.1818181818182" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="25.4545454545455" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.9090909090909" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.1818181818182" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1818181818182" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2050,81 +2534,81 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="3" ht="28" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" ht="28" spans="1:4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="4">
         <v>0.00555555555555556</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>0.0104166666666667</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="6" ht="28" spans="3:4">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="8">
+      <c r="B7" s="4">
         <v>0.0159722222222222</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="8" spans="3:3">
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="9" ht="28" spans="3:4">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1"/>
     <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="4">
         <v>0.0236111111111111</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2132,114 +2616,114 @@
       </c>
     </row>
     <row r="12" spans="3:3">
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="3:3">
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="14" ht="28" spans="3:4">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="8">
+      <c r="B15" s="4">
         <v>0.0277777777777778</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="16" ht="28" spans="3:4">
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="8">
+      <c r="B17" s="4">
         <v>0.0340277777777778</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="18" ht="28" spans="3:4">
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="8">
+      <c r="B19" s="4">
         <v>0.0409722222222222</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" ht="42" spans="3:4">
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="2:3">
-      <c r="B22" s="8">
+      <c r="B22" s="4">
         <v>0.0486111111111111</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="23" ht="28" spans="3:4">
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="1" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="24" spans="2:3">
-      <c r="B24" s="8">
+      <c r="B24" s="4">
         <v>0.0541666666666667</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="25" spans="3:4">
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1"/>
     <row r="27" spans="1:3">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="4">
         <v>0.05625</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -2247,80 +2731,80 @@
       </c>
     </row>
     <row r="28" spans="3:3">
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="29" spans="3:4">
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="30" spans="2:3">
-      <c r="B30" s="8">
+      <c r="B30" s="4">
         <v>0.0590277777777778</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="31" ht="28" spans="3:4">
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="32" spans="2:3">
-      <c r="B32" s="8">
+      <c r="B32" s="4">
         <v>0.0645833333333333</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="33" spans="3:4">
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="34" ht="28" spans="2:4">
-      <c r="B34" s="8">
+      <c r="B34" s="4">
         <v>0.06875</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="35" spans="2:3">
-      <c r="B35" s="8">
+      <c r="B35" s="4">
         <v>0.0756944444444444</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="36" spans="3:4">
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="37" s="2" customFormat="1"/>
     <row r="38" spans="1:3">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -2328,31 +2812,31 @@
       </c>
     </row>
     <row r="39" spans="3:3">
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" ht="28" spans="3:4">
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="41" ht="28" spans="3:4">
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="42" spans="3:4">
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="1" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2366,14 +2850,510 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="16.6363636363636" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.9090909090909" style="1" customWidth="1"/>
+    <col min="3" max="3" width="62" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7272727272727" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" ht="28" spans="1:3">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="4">
+        <v>0.00347222222222222</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="28" spans="2:4">
+      <c r="B6" s="4">
+        <v>0.00625</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="4">
+        <v>0.0104166666666667</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" ht="28" spans="3:4">
+      <c r="C8" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="4">
+        <v>0.0152777777777778</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3">
+      <c r="C10" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4">
+      <c r="C11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" s="2" customFormat="1"/>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.01875</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4">
+      <c r="C15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="4">
+        <v>0.0215277777777778</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="4">
+        <v>0.025</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="4"/>
+      <c r="C18" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="4">
+        <v>0.0277777777777778</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" ht="28" spans="2:4">
+      <c r="B20" s="4"/>
+      <c r="C20" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="4">
+        <v>0.0326388888888889</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4">
+      <c r="C22" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0.0354166666666667</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" ht="28" spans="3:4">
+      <c r="C26" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" s="2" customFormat="1"/>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.0409722222222222</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3">
+      <c r="C29" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4">
+      <c r="C30" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="4">
+        <v>0.0451388888888889</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4">
+      <c r="C32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="4">
+        <v>0.0486111111111111</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" ht="28" spans="3:4">
+      <c r="C34" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="4">
+        <v>0.0548611111111111</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4">
+      <c r="C36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="4">
+        <v>0.0583333333333333</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" ht="28" spans="3:4">
+      <c r="C38" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="4">
+        <v>0.0638888888888889</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" ht="28" spans="3:4">
+      <c r="C40" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" s="2" customFormat="1"/>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0.0701388888888889</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4">
+      <c r="C44" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="4">
+        <v>0.0722222222222222</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="46" ht="28" spans="3:4">
+      <c r="C46" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" s="4">
+        <v>0.0777777777777778</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" ht="28" spans="3:4">
+      <c r="C48" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="4">
+        <v>0.0826388888888889</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="C50" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="4">
+        <v>0.0861111111111111</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" ht="28" spans="3:4">
+      <c r="C52" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" s="4">
+        <v>0.0923611111111111</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4">
+      <c r="C54" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" s="2" customFormat="1"/>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="4">
+        <v>0.0951388888888889</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" ht="28" spans="3:4">
+      <c r="C58" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" ht="28" spans="2:4">
+      <c r="B59" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="B60" s="4">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
+      <c r="B61" s="4">
+        <v>0.107638888888889</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -2383,14 +3363,606 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="17.6363636363636" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" customWidth="1"/>
+    <col min="3" max="3" width="72.7272727272727" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6363636363636" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.72727272727273" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" ht="28" spans="1:3">
+      <c r="A3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" ht="28" spans="3:4">
+      <c r="C5" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="4">
+        <v>0.00416666666666667</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="4">
+        <v>0.00763888888888889</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" ht="28" spans="2:4">
+      <c r="B8" s="4">
+        <v>0.0118055555555556</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="4">
+        <v>0.0159722222222222</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4">
+      <c r="C10" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="4">
+        <v>0.01875</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" s="2" customFormat="1"/>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.0222222222222222</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3">
+      <c r="C14" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4">
+      <c r="C15" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="4">
+        <v>0.0263888888888889</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="4">
+        <v>0.0284722222222222</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="4">
+        <v>0.03125</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" ht="28" spans="2:4">
+      <c r="B20" s="4">
+        <v>0.0347222222222222</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="1"/>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.0395833333333333</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4">
+      <c r="C24" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="4">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="4">
+        <v>0.0430555555555556</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4">
+      <c r="C27" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="4">
+        <v>0.0465277777777778</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" ht="28" spans="3:4">
+      <c r="C29" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="4">
+        <v>0.0520833333333333</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4">
+      <c r="C31" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="4">
+        <v>0.0548611111111111</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4">
+      <c r="C33" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="4">
+        <v>0.0590277777777778</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4">
+      <c r="C37" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="4">
+        <v>0.0631944444444444</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" ht="28" spans="3:4">
+      <c r="C39" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="4">
+        <v>0.0673611111111111</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4">
+      <c r="C41" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" s="4">
+        <v>0.0694444444444444</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" s="4">
+        <v>0.0736111111111111</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4">
+      <c r="C46" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" s="4">
+        <v>0.0770833333333333</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" ht="28" spans="3:4">
+      <c r="C48" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="4">
+        <v>0.0819444444444444</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="50" ht="28" spans="3:4">
+      <c r="C50" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="4">
+        <v>0.0881944444444444</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="52" ht="28" spans="3:4">
+      <c r="C52" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" s="4">
+        <v>0.09375</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4">
+      <c r="C54" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" s="4">
+        <v>0.0979166666666667</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4">
+      <c r="C56" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="57" s="2" customFormat="1"/>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="4">
+        <v>0.102083333333333</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4">
+      <c r="C60" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" s="4">
+        <v>0.105555555555556</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4">
+      <c r="C62" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" s="4">
+        <v>0.107638888888889</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4">
+      <c r="C64" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" s="4">
+        <v>0.109027777777778</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4">
+      <c r="C66" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" s="4">
+        <v>0.111805555555556</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" spans="2:3">
+      <c r="B69" s="4">
+        <v>0.113194444444444</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="70" ht="28" spans="3:4">
+      <c r="C70" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="71" ht="28" spans="2:4">
+      <c r="B71" s="4">
+        <v>0.118055555555556</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="B72" s="4">
+        <v>0.123611111111111</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>